<commit_message>
table creation fully set up
</commit_message>
<xml_diff>
--- a/Output/Modelling/Logistic Regression/Tables/exclude_previous_Most_Complex_Model_Classification_Report.xlsx
+++ b/Output/Modelling/Logistic Regression/Tables/exclude_previous_Most_Complex_Model_Classification_Report.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.6793</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.84</t>
+          <t>0.5841</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.6281</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>214</t>
         </is>
       </c>
     </row>
@@ -495,76 +495,76 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.5882</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.33</t>
+          <t>0.4762</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>0.5263</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>42</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.63</t>
+          <t>0.7917</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.54</t>
+          <t>0.7037</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>0.7451</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>27</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>0.5822</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.6159</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.66</t>
+          <t>0.5986</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>138</t>
         </is>
       </c>
     </row>
@@ -576,76 +576,76 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.60</t>
+          <t>0.6399</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.6678</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.6535</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>298</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.60</t>
+          <t>0.6759</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.7416</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.53</t>
+          <t>0.7072</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>329</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.60</t>
+          <t>0.7778</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.22</t>
+          <t>1.0000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.32</t>
+          <t>0.8750</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -657,49 +657,49 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.8095</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.5000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.6182</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>34</t>
         </is>
       </c>
     </row>
@@ -711,22 +711,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix classification report sort order
</commit_message>
<xml_diff>
--- a/Output/Modelling/Logistic Regression/Tables/exclude_previous_Most_Complex_Model_Classification_Report.xlsx
+++ b/Output/Modelling/Logistic Regression/Tables/exclude_previous_Most_Complex_Model_Classification_Report.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.5874</t>
+          <t>0.8261</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.6298</t>
+          <t>0.7917</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.6079</t>
+          <t>0.8085</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>24</t>
         </is>
       </c>
     </row>
@@ -517,54 +517,54 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.8261</t>
+          <t>0.5874</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.7917</t>
+          <t>0.6298</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.8085</t>
+          <t>0.6079</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>208</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.5864</t>
+          <t>0.6909</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.7273</t>
+          <t>0.6281</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.6493</t>
+          <t>0.6580</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>363</t>
         </is>
       </c>
     </row>
@@ -598,54 +598,54 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.6909</t>
+          <t>0.5864</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.6281</t>
+          <t>0.7273</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.6580</t>
+          <t>0.6493</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>363</t>
+          <t>154</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.0000</t>
+          <t>0.5556</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0000</t>
+          <t>0.7692</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.0000</t>
+          <t>0.6452</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>26</t>
         </is>
       </c>
     </row>
@@ -679,27 +679,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.5556</t>
+          <t>1.0000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.7692</t>
+          <t>1.0000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.6452</t>
+          <t>1.0000</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>